<commit_message>
Batch size experiment analysis
</commit_message>
<xml_diff>
--- a/tests/batch_size_experiment/batch_size_experiment_results.xlsx
+++ b/tests/batch_size_experiment/batch_size_experiment_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>train_size</t>
   </si>
@@ -104,6 +104,36 @@
   </si>
   <si>
     <t>0:20:39</t>
+  </si>
+  <si>
+    <t>0:09:10</t>
+  </si>
+  <si>
+    <t>0:34:37</t>
+  </si>
+  <si>
+    <t>0:22:46</t>
+  </si>
+  <si>
+    <t>0:16:53</t>
+  </si>
+  <si>
+    <t>0:09:29</t>
+  </si>
+  <si>
+    <t>0:14:34</t>
+  </si>
+  <si>
+    <t>0:44:18</t>
+  </si>
+  <si>
+    <t>0:23:21</t>
+  </si>
+  <si>
+    <t>0:15:10</t>
+  </si>
+  <si>
+    <t>0:08:44</t>
   </si>
 </sst>
 </file>
@@ -461,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -909,6 +939,176 @@
         <v>29</v>
       </c>
     </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>500</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0.337386018237082</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>500</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>0.3399735878823331</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>500</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>0.8538578986332499</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>500</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>0.8690897597977244</v>
+      </c>
+      <c r="D30">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>500</v>
+      </c>
+      <c r="B31">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>0.8583499539481968</v>
+      </c>
+      <c r="D31">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>300</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0.337386018237082</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>300</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>0.8236784407325322</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>300</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>0.8551013625789299</v>
+      </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>300</v>
+      </c>
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <v>0.8222474726552276</v>
+      </c>
+      <c r="D35">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>300</v>
+      </c>
+      <c r="B36">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>0.8124270846989434</v>
+      </c>
+      <c r="D36">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>